<commit_message>
added dropdown for output dialog
</commit_message>
<xml_diff>
--- a/data/Em3/PrBlank.xlsx
+++ b/data/Em3/PrBlank.xlsx
@@ -47,13 +47,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -84,7 +90,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>